<commit_message>
Merged PR 7442: PRI-19856 Export Campaign to Excel - Add ADUs to Flow Chart Tab
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/Stub Advertiser DAY EMN MDN PA PT Q4'19-Q2'20 Plan Rev - 12-16.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/Stub Advertiser DAY EMN MDN PA PT Q4'19-Q2'20 Plan Rev - 12-16.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -241,6 +241,9 @@
     <t>4Q '19 PT Total</t>
   </si>
   <si>
+    <t>4Q '19 ADU</t>
+  </si>
+  <si>
     <t xml:space="preserve">1Q '20 MDN :90s </t>
   </si>
   <si>
@@ -274,6 +277,9 @@
     <t>1Q '20 EMN Total</t>
   </si>
   <si>
+    <t>1Q '20 ADU</t>
+  </si>
+  <si>
     <t xml:space="preserve">2Q '20 MDN :90s </t>
   </si>
   <si>
@@ -295,6 +301,9 @@
     <t>2Q '20 PA Total</t>
   </si>
   <si>
+    <t>2Q '20 ADU</t>
+  </si>
+  <si>
     <t>:15 equiv., :30</t>
   </si>
   <si>
@@ -307,7 +316,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 02/10/20</t>
+    <t>Created 02/14/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -1837,7 +1846,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:P185"/>
+  <dimension ref="A2:P212"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0" tabSelected="0">
       <selection activeCell="C15" sqref="C15"/>
@@ -2119,10 +2128,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="P11" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="12" ht="24" customHeight="1" s="94" customFormat="1">
@@ -2213,10 +2222,10 @@
         <v>0</v>
       </c>
       <c r="O13" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
       <c r="P13" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1" s="94" customFormat="1">
@@ -2447,10 +2456,10 @@
         <v>0</v>
       </c>
       <c r="O20" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="P20" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="21" ht="24" customHeight="1">
@@ -2541,10 +2550,10 @@
         <v>0</v>
       </c>
       <c r="O22" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
       <c r="P22" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
@@ -2775,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="O29" s="98">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="P29" s="98">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="30" ht="24" customHeight="1">
@@ -2869,10 +2878,10 @@
         <v>0</v>
       </c>
       <c r="O31" s="63">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="P31" s="63">
-        <v>250000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="32" ht="30" customHeight="1">
@@ -3103,10 +3112,10 @@
         <v>0</v>
       </c>
       <c r="O38" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="P38" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="39" ht="24" customHeight="1">
@@ -3197,10 +3206,10 @@
         <v>0</v>
       </c>
       <c r="O40" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
       <c r="P40" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="41" ht="30" customHeight="1">
@@ -3431,10 +3440,10 @@
         <v>0</v>
       </c>
       <c r="O47" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="P47" s="98">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="48" ht="24" customHeight="1">
@@ -3525,10 +3534,10 @@
         <v>0</v>
       </c>
       <c r="O49" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
       <c r="P49" s="63">
-        <v>125000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="50" ht="30" customHeight="1">
@@ -3759,10 +3768,10 @@
         <v>0</v>
       </c>
       <c r="O56" s="98">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="P56" s="98">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="57" ht="24" customHeight="1">
@@ -3853,10 +3862,10 @@
         <v>0</v>
       </c>
       <c r="O58" s="63">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="P58" s="63">
-        <v>250000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="59" ht="30" customHeight="1">
@@ -4542,19 +4551,19 @@
         <v>69</v>
       </c>
       <c r="C79" s="133" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D79" s="133"/>
       <c r="E79" s="133"/>
       <c r="F79" s="134"/>
       <c r="G79" s="133" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H79" s="133"/>
       <c r="I79" s="133"/>
       <c r="J79" s="134"/>
       <c r="K79" s="135" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="L79" s="133"/>
       <c r="M79" s="133"/>
@@ -4566,43 +4575,43 @@
       <c r="A80" s="57"/>
       <c r="B80" s="66"/>
       <c r="C80" s="55">
-        <v>43829</v>
+        <v>43738</v>
       </c>
       <c r="D80" s="55">
-        <v>43836</v>
+        <v>43745</v>
       </c>
       <c r="E80" s="55">
-        <v>43843</v>
+        <v>43752</v>
       </c>
       <c r="F80" s="56">
-        <v>43850</v>
+        <v>43759</v>
       </c>
       <c r="G80" s="55">
-        <v>43857</v>
+        <v>43766</v>
       </c>
       <c r="H80" s="55">
-        <v>43864</v>
+        <v>43773</v>
       </c>
       <c r="I80" s="55">
-        <v>43871</v>
+        <v>43780</v>
       </c>
       <c r="J80" s="56">
-        <v>43878</v>
+        <v>43787</v>
       </c>
       <c r="K80" s="55">
-        <v>43885</v>
+        <v>43794</v>
       </c>
       <c r="L80" s="55">
-        <v>43892</v>
+        <v>43801</v>
       </c>
       <c r="M80" s="55">
-        <v>43899</v>
+        <v>43808</v>
       </c>
       <c r="N80" s="55">
-        <v>43906</v>
+        <v>43815</v>
       </c>
       <c r="O80" s="56">
-        <v>43913</v>
+        <v>43822</v>
       </c>
       <c r="P80" s="60" t="s">
         <v>37</v>
@@ -4612,45 +4621,19 @@
       <c r="B81" s="114" t="s">
         <v>58</v>
       </c>
-      <c r="C81" s="101">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="D81" s="102">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="E81" s="102">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="F81" s="59">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="G81" s="101">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="H81" s="102">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="I81" s="102">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="J81" s="59">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="K81" s="101">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="L81" s="102">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="M81" s="102">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="N81" s="102">
-        <v>0.019230769230769232</v>
-      </c>
-      <c r="O81" s="59">
-        <v>0.019230769230769232</v>
-      </c>
+      <c r="C81" s="101"/>
+      <c r="D81" s="102"/>
+      <c r="E81" s="102"/>
+      <c r="F81" s="59"/>
+      <c r="G81" s="101"/>
+      <c r="H81" s="102"/>
+      <c r="I81" s="102"/>
+      <c r="J81" s="59"/>
+      <c r="K81" s="101"/>
+      <c r="L81" s="102"/>
+      <c r="M81" s="102"/>
+      <c r="N81" s="102"/>
+      <c r="O81" s="59"/>
       <c r="P81" s="105" t="s">
         <v>38</v>
       </c>
@@ -4659,189 +4642,77 @@
       <c r="B82" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="C82" s="104">
-        <v>0</v>
-      </c>
-      <c r="D82" s="96">
-        <v>0</v>
-      </c>
-      <c r="E82" s="106">
-        <v>0</v>
-      </c>
-      <c r="F82" s="107">
-        <v>0</v>
-      </c>
-      <c r="G82" s="104">
-        <v>0</v>
-      </c>
-      <c r="H82" s="96">
-        <v>0</v>
-      </c>
-      <c r="I82" s="106">
-        <v>0</v>
-      </c>
-      <c r="J82" s="107">
-        <v>0</v>
-      </c>
-      <c r="K82" s="104">
-        <v>0</v>
-      </c>
-      <c r="L82" s="96">
-        <v>0</v>
-      </c>
-      <c r="M82" s="106">
-        <v>0</v>
-      </c>
-      <c r="N82" s="106">
-        <v>0</v>
-      </c>
-      <c r="O82" s="99">
-        <v>0</v>
-      </c>
-      <c r="P82" s="99">
-        <v>0</v>
-      </c>
+      <c r="C82" s="104"/>
+      <c r="D82" s="96"/>
+      <c r="E82" s="106"/>
+      <c r="F82" s="107"/>
+      <c r="G82" s="104"/>
+      <c r="H82" s="96"/>
+      <c r="I82" s="106"/>
+      <c r="J82" s="107"/>
+      <c r="K82" s="104"/>
+      <c r="L82" s="96"/>
+      <c r="M82" s="106"/>
+      <c r="N82" s="106"/>
+      <c r="O82" s="99"/>
+      <c r="P82" s="99"/>
     </row>
     <row r="83" ht="24" customHeight="1">
       <c r="B83" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="C83" s="103">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="D83" s="95">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="E83" s="108">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="F83" s="109">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="G83" s="103">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="H83" s="95">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="I83" s="108">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="J83" s="109">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="K83" s="103">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="L83" s="95">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="M83" s="108">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="N83" s="108">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="O83" s="98">
-        <v>384.61538461538464</v>
-      </c>
-      <c r="P83" s="98">
-        <v>5000.0000000000036</v>
-      </c>
+      <c r="C83" s="103"/>
+      <c r="D83" s="95"/>
+      <c r="E83" s="108"/>
+      <c r="F83" s="109"/>
+      <c r="G83" s="103"/>
+      <c r="H83" s="95"/>
+      <c r="I83" s="108"/>
+      <c r="J83" s="109"/>
+      <c r="K83" s="103"/>
+      <c r="L83" s="95"/>
+      <c r="M83" s="108"/>
+      <c r="N83" s="108"/>
+      <c r="O83" s="98"/>
+      <c r="P83" s="98"/>
     </row>
     <row r="84" ht="24" customHeight="1">
       <c r="B84" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="C84" s="110">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="D84" s="97">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="E84" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="F84" s="112">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="G84" s="110">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="H84" s="97">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="I84" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="J84" s="112">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="K84" s="110">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="L84" s="97">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="M84" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="N84" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="O84" s="113">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="P84" s="113">
-        <v>24.999999999999957</v>
-      </c>
+      <c r="C84" s="110"/>
+      <c r="D84" s="97"/>
+      <c r="E84" s="111"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="110"/>
+      <c r="H84" s="97"/>
+      <c r="I84" s="111"/>
+      <c r="J84" s="112"/>
+      <c r="K84" s="110"/>
+      <c r="L84" s="97"/>
+      <c r="M84" s="111"/>
+      <c r="N84" s="111"/>
+      <c r="O84" s="113"/>
+      <c r="P84" s="113"/>
     </row>
     <row r="85" ht="24" customHeight="1">
       <c r="B85" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="C85" s="61">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="D85" s="62">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="E85" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="F85" s="65">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="G85" s="61">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="H85" s="62">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="I85" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="J85" s="65">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="K85" s="61">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="L85" s="62">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="M85" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="N85" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="O85" s="63">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="P85" s="63">
-        <v>124999.9999999998</v>
-      </c>
+      <c r="C85" s="61"/>
+      <c r="D85" s="62"/>
+      <c r="E85" s="64"/>
+      <c r="F85" s="65"/>
+      <c r="G85" s="61"/>
+      <c r="H85" s="62"/>
+      <c r="I85" s="64"/>
+      <c r="J85" s="65"/>
+      <c r="K85" s="61"/>
+      <c r="L85" s="62"/>
+      <c r="M85" s="64"/>
+      <c r="N85" s="64"/>
+      <c r="O85" s="63"/>
+      <c r="P85" s="63"/>
     </row>
     <row r="86" ht="30" customHeight="1">
       <c r="B86" s="116" t="s">
@@ -4860,29 +4731,27 @@
       <c r="M86" s="118"/>
       <c r="N86" s="118"/>
       <c r="O86" s="119"/>
-      <c r="P86" s="120">
-        <v>0</v>
-      </c>
+      <c r="P86" s="120"/>
     </row>
     <row r="88">
       <c r="A88" s="57"/>
       <c r="B88" s="67" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C88" s="133" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D88" s="133"/>
       <c r="E88" s="133"/>
       <c r="F88" s="134"/>
       <c r="G88" s="133" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H88" s="133"/>
       <c r="I88" s="133"/>
       <c r="J88" s="134"/>
       <c r="K88" s="135" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L88" s="133"/>
       <c r="M88" s="133"/>
@@ -4941,43 +4810,43 @@
         <v>58</v>
       </c>
       <c r="C90" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="D90" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="E90" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="F90" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="G90" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="H90" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="I90" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="J90" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="K90" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="L90" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="M90" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="N90" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="O90" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="P90" s="105" t="s">
         <v>38</v>
@@ -5035,46 +4904,46 @@
         <v>59</v>
       </c>
       <c r="C92" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="D92" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="E92" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="F92" s="109">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="G92" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="H92" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="I92" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="J92" s="109">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="K92" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="L92" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="M92" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="N92" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="O92" s="98">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="P92" s="98">
-        <v>5000.0000000000036</v>
+        <v>5000.0000000000009</v>
       </c>
     </row>
     <row r="93" ht="24" customHeight="1">
@@ -5198,19 +5067,19 @@
         <v>74</v>
       </c>
       <c r="C97" s="133" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D97" s="133"/>
       <c r="E97" s="133"/>
       <c r="F97" s="134"/>
       <c r="G97" s="133" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H97" s="133"/>
       <c r="I97" s="133"/>
       <c r="J97" s="134"/>
       <c r="K97" s="135" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L97" s="133"/>
       <c r="M97" s="133"/>
@@ -5402,7 +5271,7 @@
         <v>384.61538461538464</v>
       </c>
       <c r="P101" s="98">
-        <v>5000.0000000000036</v>
+        <v>5000.0000000000009</v>
       </c>
     </row>
     <row r="102" ht="24" customHeight="1">
@@ -5526,19 +5395,19 @@
         <v>75</v>
       </c>
       <c r="C106" s="133" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D106" s="133"/>
       <c r="E106" s="133"/>
       <c r="F106" s="134"/>
       <c r="G106" s="133" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H106" s="133"/>
       <c r="I106" s="133"/>
       <c r="J106" s="134"/>
       <c r="K106" s="135" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L106" s="133"/>
       <c r="M106" s="133"/>
@@ -5597,43 +5466,43 @@
         <v>58</v>
       </c>
       <c r="C108" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="D108" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="E108" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="F108" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="G108" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="H108" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="I108" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="J108" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="K108" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="L108" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="M108" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="N108" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="O108" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="P108" s="105" t="s">
         <v>38</v>
@@ -5691,46 +5560,46 @@
         <v>59</v>
       </c>
       <c r="C110" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="D110" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="E110" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="F110" s="109">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="G110" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="H110" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="I110" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="J110" s="109">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="K110" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="L110" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="M110" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="N110" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="O110" s="98">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="P110" s="98">
-        <v>5000.0000000000036</v>
+        <v>5000.0000000000009</v>
       </c>
     </row>
     <row r="111" ht="24" customHeight="1">
@@ -5854,19 +5723,19 @@
         <v>76</v>
       </c>
       <c r="C115" s="133" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D115" s="133"/>
       <c r="E115" s="133"/>
       <c r="F115" s="134"/>
       <c r="G115" s="133" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H115" s="133"/>
       <c r="I115" s="133"/>
       <c r="J115" s="134"/>
       <c r="K115" s="135" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L115" s="133"/>
       <c r="M115" s="133"/>
@@ -5925,43 +5794,43 @@
         <v>58</v>
       </c>
       <c r="C117" s="101">
-        <v>0.25</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="D117" s="102">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="E117" s="102">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="F117" s="59">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="G117" s="101">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="H117" s="102">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="I117" s="102">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="J117" s="59">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="K117" s="101">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="L117" s="102">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="M117" s="102">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="N117" s="102">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="O117" s="59">
-        <v>0</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="P117" s="105" t="s">
         <v>38</v>
@@ -6019,46 +5888,46 @@
         <v>59</v>
       </c>
       <c r="C119" s="103">
-        <v>5000</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="D119" s="95">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="E119" s="108">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="F119" s="109">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="G119" s="103">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="H119" s="95">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="I119" s="108">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="J119" s="109">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="K119" s="103">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="L119" s="95">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="M119" s="108">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="N119" s="108">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="O119" s="98">
-        <v>0</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="P119" s="98">
-        <v>5000</v>
+        <v>5000.0000000000009</v>
       </c>
     </row>
     <row r="120" ht="24" customHeight="1">
@@ -6066,46 +5935,46 @@
         <v>30</v>
       </c>
       <c r="C120" s="110">
-        <v>25</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="D120" s="97">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="E120" s="111">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="F120" s="112">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="G120" s="110">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="H120" s="97">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="I120" s="111">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="J120" s="112">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="K120" s="110">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="L120" s="97">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="M120" s="111">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="N120" s="111">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="O120" s="113">
-        <v>0</v>
+        <v>24.999999999999936</v>
       </c>
       <c r="P120" s="113">
-        <v>25</v>
+        <v>24.999999999999957</v>
       </c>
     </row>
     <row r="121" ht="24" customHeight="1">
@@ -6113,46 +5982,46 @@
         <v>60</v>
       </c>
       <c r="C121" s="61">
-        <v>125000</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="D121" s="62">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="E121" s="64">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="F121" s="65">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="G121" s="61">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="H121" s="62">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="I121" s="64">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="J121" s="65">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="K121" s="61">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="L121" s="62">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="M121" s="64">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="N121" s="64">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="O121" s="63">
-        <v>0</v>
+        <v>9615.3846153846</v>
       </c>
       <c r="P121" s="63">
-        <v>125000</v>
+        <v>124999.9999999998</v>
       </c>
     </row>
     <row r="122" ht="30" customHeight="1">
@@ -6182,19 +6051,19 @@
         <v>77</v>
       </c>
       <c r="C124" s="133" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D124" s="133"/>
       <c r="E124" s="133"/>
       <c r="F124" s="134"/>
       <c r="G124" s="133" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H124" s="133"/>
       <c r="I124" s="133"/>
       <c r="J124" s="134"/>
       <c r="K124" s="135" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L124" s="133"/>
       <c r="M124" s="133"/>
@@ -6510,19 +6379,19 @@
         <v>78</v>
       </c>
       <c r="C133" s="133" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D133" s="133"/>
       <c r="E133" s="133"/>
       <c r="F133" s="134"/>
       <c r="G133" s="133" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H133" s="133"/>
       <c r="I133" s="133"/>
       <c r="J133" s="134"/>
       <c r="K133" s="135" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L133" s="133"/>
       <c r="M133" s="133"/>
@@ -6838,19 +6707,19 @@
         <v>79</v>
       </c>
       <c r="C142" s="133" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D142" s="133"/>
       <c r="E142" s="133"/>
       <c r="F142" s="134"/>
       <c r="G142" s="133" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H142" s="133"/>
       <c r="I142" s="133"/>
       <c r="J142" s="134"/>
       <c r="K142" s="135" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L142" s="133"/>
       <c r="M142" s="133"/>
@@ -7166,19 +7035,19 @@
         <v>80</v>
       </c>
       <c r="C151" s="133" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D151" s="133"/>
       <c r="E151" s="133"/>
       <c r="F151" s="134"/>
       <c r="G151" s="133" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H151" s="133"/>
       <c r="I151" s="133"/>
       <c r="J151" s="134"/>
       <c r="K151" s="135" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="L151" s="133"/>
       <c r="M151" s="133"/>
@@ -7190,43 +7059,43 @@
       <c r="A152" s="57"/>
       <c r="B152" s="66"/>
       <c r="C152" s="55">
-        <v>43920</v>
+        <v>43829</v>
       </c>
       <c r="D152" s="55">
-        <v>43927</v>
+        <v>43836</v>
       </c>
       <c r="E152" s="55">
-        <v>43934</v>
+        <v>43843</v>
       </c>
       <c r="F152" s="56">
-        <v>43941</v>
+        <v>43850</v>
       </c>
       <c r="G152" s="55">
-        <v>43948</v>
+        <v>43857</v>
       </c>
       <c r="H152" s="55">
-        <v>43955</v>
+        <v>43864</v>
       </c>
       <c r="I152" s="55">
-        <v>43962</v>
+        <v>43871</v>
       </c>
       <c r="J152" s="56">
-        <v>43969</v>
+        <v>43878</v>
       </c>
       <c r="K152" s="55">
-        <v>43976</v>
+        <v>43885</v>
       </c>
       <c r="L152" s="55">
-        <v>43983</v>
+        <v>43892</v>
       </c>
       <c r="M152" s="55">
-        <v>43990</v>
+        <v>43899</v>
       </c>
       <c r="N152" s="55">
-        <v>43997</v>
+        <v>43906</v>
       </c>
       <c r="O152" s="56">
-        <v>44004</v>
+        <v>43913</v>
       </c>
       <c r="P152" s="60" t="s">
         <v>37</v>
@@ -7237,43 +7106,43 @@
         <v>58</v>
       </c>
       <c r="C153" s="101">
-        <v>0.019230769230769232</v>
+        <v>0.25</v>
       </c>
       <c r="D153" s="102">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="E153" s="102">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="F153" s="59">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="G153" s="101">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="H153" s="102">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="I153" s="102">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="J153" s="59">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="K153" s="101">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="L153" s="102">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="M153" s="102">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="N153" s="102">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="O153" s="59">
-        <v>0.019230769230769232</v>
+        <v>0</v>
       </c>
       <c r="P153" s="105" t="s">
         <v>38</v>
@@ -7331,46 +7200,46 @@
         <v>59</v>
       </c>
       <c r="C155" s="103">
-        <v>384.61538461538464</v>
+        <v>5000</v>
       </c>
       <c r="D155" s="95">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="E155" s="108">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="F155" s="109">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="G155" s="103">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="H155" s="95">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="I155" s="108">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="J155" s="109">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="K155" s="103">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="L155" s="95">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="M155" s="108">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="N155" s="108">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="O155" s="98">
-        <v>384.61538461538464</v>
+        <v>0</v>
       </c>
       <c r="P155" s="98">
-        <v>5000.0000000000036</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="156" ht="24" customHeight="1">
@@ -7378,46 +7247,46 @@
         <v>30</v>
       </c>
       <c r="C156" s="110">
-        <v>24.999999999999936</v>
+        <v>25</v>
       </c>
       <c r="D156" s="97">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="E156" s="111">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="F156" s="112">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="G156" s="110">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="H156" s="97">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="I156" s="111">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="J156" s="112">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="K156" s="110">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="L156" s="97">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="M156" s="111">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="N156" s="111">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="O156" s="113">
-        <v>24.999999999999936</v>
+        <v>0</v>
       </c>
       <c r="P156" s="113">
-        <v>24.999999999999957</v>
+        <v>25</v>
       </c>
     </row>
     <row r="157" ht="24" customHeight="1">
@@ -7425,46 +7294,46 @@
         <v>60</v>
       </c>
       <c r="C157" s="61">
-        <v>9615.3846153846</v>
+        <v>125000</v>
       </c>
       <c r="D157" s="62">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="E157" s="64">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="F157" s="65">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="G157" s="61">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="H157" s="62">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="I157" s="64">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="J157" s="65">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="K157" s="61">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="L157" s="62">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="M157" s="64">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="N157" s="64">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="O157" s="63">
-        <v>9615.3846153846</v>
+        <v>0</v>
       </c>
       <c r="P157" s="63">
-        <v>124999.9999999998</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="158" ht="30" customHeight="1">
@@ -7491,22 +7360,22 @@
     <row r="160">
       <c r="A160" s="57"/>
       <c r="B160" s="67" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C160" s="133" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D160" s="133"/>
       <c r="E160" s="133"/>
       <c r="F160" s="134"/>
       <c r="G160" s="133" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H160" s="133"/>
       <c r="I160" s="133"/>
       <c r="J160" s="134"/>
       <c r="K160" s="135" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="L160" s="133"/>
       <c r="M160" s="133"/>
@@ -7518,43 +7387,43 @@
       <c r="A161" s="57"/>
       <c r="B161" s="66"/>
       <c r="C161" s="55">
-        <v>43920</v>
+        <v>43829</v>
       </c>
       <c r="D161" s="55">
-        <v>43927</v>
+        <v>43836</v>
       </c>
       <c r="E161" s="55">
-        <v>43934</v>
+        <v>43843</v>
       </c>
       <c r="F161" s="56">
-        <v>43941</v>
+        <v>43850</v>
       </c>
       <c r="G161" s="55">
-        <v>43948</v>
+        <v>43857</v>
       </c>
       <c r="H161" s="55">
-        <v>43955</v>
+        <v>43864</v>
       </c>
       <c r="I161" s="55">
-        <v>43962</v>
+        <v>43871</v>
       </c>
       <c r="J161" s="56">
-        <v>43969</v>
+        <v>43878</v>
       </c>
       <c r="K161" s="55">
-        <v>43976</v>
+        <v>43885</v>
       </c>
       <c r="L161" s="55">
-        <v>43983</v>
+        <v>43892</v>
       </c>
       <c r="M161" s="55">
-        <v>43990</v>
+        <v>43899</v>
       </c>
       <c r="N161" s="55">
-        <v>43997</v>
+        <v>43906</v>
       </c>
       <c r="O161" s="56">
-        <v>44004</v>
+        <v>43913</v>
       </c>
       <c r="P161" s="60" t="s">
         <v>37</v>
@@ -7564,45 +7433,19 @@
       <c r="B162" s="114" t="s">
         <v>58</v>
       </c>
-      <c r="C162" s="101">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="D162" s="102">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="E162" s="102">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="F162" s="59">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="G162" s="101">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="H162" s="102">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="I162" s="102">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="J162" s="59">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="K162" s="101">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="L162" s="102">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="M162" s="102">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="N162" s="102">
-        <v>0.0192307692307692</v>
-      </c>
-      <c r="O162" s="59">
-        <v>0.0192307692307692</v>
-      </c>
+      <c r="C162" s="101"/>
+      <c r="D162" s="102"/>
+      <c r="E162" s="102"/>
+      <c r="F162" s="59"/>
+      <c r="G162" s="101"/>
+      <c r="H162" s="102"/>
+      <c r="I162" s="102"/>
+      <c r="J162" s="59"/>
+      <c r="K162" s="101"/>
+      <c r="L162" s="102"/>
+      <c r="M162" s="102"/>
+      <c r="N162" s="102"/>
+      <c r="O162" s="59"/>
       <c r="P162" s="105" t="s">
         <v>38</v>
       </c>
@@ -7611,189 +7454,77 @@
       <c r="B163" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="C163" s="104">
-        <v>0</v>
-      </c>
-      <c r="D163" s="96">
-        <v>0</v>
-      </c>
-      <c r="E163" s="106">
-        <v>0</v>
-      </c>
-      <c r="F163" s="107">
-        <v>0</v>
-      </c>
-      <c r="G163" s="104">
-        <v>0</v>
-      </c>
-      <c r="H163" s="96">
-        <v>0</v>
-      </c>
-      <c r="I163" s="106">
-        <v>0</v>
-      </c>
-      <c r="J163" s="107">
-        <v>0</v>
-      </c>
-      <c r="K163" s="104">
-        <v>0</v>
-      </c>
-      <c r="L163" s="96">
-        <v>0</v>
-      </c>
-      <c r="M163" s="106">
-        <v>0</v>
-      </c>
-      <c r="N163" s="106">
-        <v>0</v>
-      </c>
-      <c r="O163" s="99">
-        <v>0</v>
-      </c>
-      <c r="P163" s="99">
-        <v>0</v>
-      </c>
+      <c r="C163" s="104"/>
+      <c r="D163" s="96"/>
+      <c r="E163" s="106"/>
+      <c r="F163" s="107"/>
+      <c r="G163" s="104"/>
+      <c r="H163" s="96"/>
+      <c r="I163" s="106"/>
+      <c r="J163" s="107"/>
+      <c r="K163" s="104"/>
+      <c r="L163" s="96"/>
+      <c r="M163" s="106"/>
+      <c r="N163" s="106"/>
+      <c r="O163" s="99"/>
+      <c r="P163" s="99"/>
     </row>
     <row r="164" ht="24" customHeight="1">
       <c r="B164" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="C164" s="103">
-        <v>384.615384615385</v>
-      </c>
-      <c r="D164" s="95">
-        <v>384.615384615385</v>
-      </c>
-      <c r="E164" s="108">
-        <v>384.615384615385</v>
-      </c>
-      <c r="F164" s="109">
-        <v>384.615384615385</v>
-      </c>
-      <c r="G164" s="103">
-        <v>384.615384615385</v>
-      </c>
-      <c r="H164" s="95">
-        <v>384.615384615385</v>
-      </c>
-      <c r="I164" s="108">
-        <v>384.615384615385</v>
-      </c>
-      <c r="J164" s="109">
-        <v>384.615384615385</v>
-      </c>
-      <c r="K164" s="103">
-        <v>384.615384615385</v>
-      </c>
-      <c r="L164" s="95">
-        <v>384.615384615385</v>
-      </c>
-      <c r="M164" s="108">
-        <v>384.615384615385</v>
-      </c>
-      <c r="N164" s="108">
-        <v>384.615384615385</v>
-      </c>
-      <c r="O164" s="98">
-        <v>384.615384615385</v>
-      </c>
-      <c r="P164" s="98">
-        <v>5000.0000000000036</v>
-      </c>
+      <c r="C164" s="103"/>
+      <c r="D164" s="95"/>
+      <c r="E164" s="108"/>
+      <c r="F164" s="109"/>
+      <c r="G164" s="103"/>
+      <c r="H164" s="95"/>
+      <c r="I164" s="108"/>
+      <c r="J164" s="109"/>
+      <c r="K164" s="103"/>
+      <c r="L164" s="95"/>
+      <c r="M164" s="108"/>
+      <c r="N164" s="108"/>
+      <c r="O164" s="98"/>
+      <c r="P164" s="98"/>
     </row>
     <row r="165" ht="24" customHeight="1">
       <c r="B165" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="C165" s="110">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="D165" s="97">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="E165" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="F165" s="112">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="G165" s="110">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="H165" s="97">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="I165" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="J165" s="112">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="K165" s="110">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="L165" s="97">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="M165" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="N165" s="111">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="O165" s="113">
-        <v>24.999999999999936</v>
-      </c>
-      <c r="P165" s="113">
-        <v>24.999999999999957</v>
-      </c>
+      <c r="C165" s="110"/>
+      <c r="D165" s="97"/>
+      <c r="E165" s="111"/>
+      <c r="F165" s="112"/>
+      <c r="G165" s="110"/>
+      <c r="H165" s="97"/>
+      <c r="I165" s="111"/>
+      <c r="J165" s="112"/>
+      <c r="K165" s="110"/>
+      <c r="L165" s="97"/>
+      <c r="M165" s="111"/>
+      <c r="N165" s="111"/>
+      <c r="O165" s="113"/>
+      <c r="P165" s="113"/>
     </row>
     <row r="166" ht="24" customHeight="1">
       <c r="B166" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="C166" s="61">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="D166" s="62">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="E166" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="F166" s="65">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="G166" s="61">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="H166" s="62">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="I166" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="J166" s="65">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="K166" s="61">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="L166" s="62">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="M166" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="N166" s="64">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="O166" s="63">
-        <v>9615.3846153846</v>
-      </c>
-      <c r="P166" s="63">
-        <v>124999.9999999998</v>
-      </c>
+      <c r="C166" s="61"/>
+      <c r="D166" s="62"/>
+      <c r="E166" s="64"/>
+      <c r="F166" s="65"/>
+      <c r="G166" s="61"/>
+      <c r="H166" s="62"/>
+      <c r="I166" s="64"/>
+      <c r="J166" s="65"/>
+      <c r="K166" s="61"/>
+      <c r="L166" s="62"/>
+      <c r="M166" s="64"/>
+      <c r="N166" s="64"/>
+      <c r="O166" s="63"/>
+      <c r="P166" s="63"/>
     </row>
     <row r="167" ht="30" customHeight="1">
       <c r="B167" s="116" t="s">
@@ -7812,29 +7543,27 @@
       <c r="M167" s="118"/>
       <c r="N167" s="118"/>
       <c r="O167" s="119"/>
-      <c r="P167" s="120">
-        <v>0</v>
-      </c>
+      <c r="P167" s="120"/>
     </row>
     <row r="169">
       <c r="A169" s="57"/>
       <c r="B169" s="67" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C169" s="133" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D169" s="133"/>
       <c r="E169" s="133"/>
       <c r="F169" s="134"/>
       <c r="G169" s="133" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H169" s="133"/>
       <c r="I169" s="133"/>
       <c r="J169" s="134"/>
       <c r="K169" s="135" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L169" s="133"/>
       <c r="M169" s="133"/>
@@ -8026,7 +7755,7 @@
         <v>384.61538461538464</v>
       </c>
       <c r="P173" s="98">
-        <v>5000.0000000000036</v>
+        <v>5000.0000000000009</v>
       </c>
     </row>
     <row r="174" ht="24" customHeight="1">
@@ -8150,19 +7879,19 @@
         <v>86</v>
       </c>
       <c r="C178" s="133" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D178" s="133"/>
       <c r="E178" s="133"/>
       <c r="F178" s="134"/>
       <c r="G178" s="133" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H178" s="133"/>
       <c r="I178" s="133"/>
       <c r="J178" s="134"/>
       <c r="K178" s="135" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L178" s="133"/>
       <c r="M178" s="133"/>
@@ -8221,43 +7950,43 @@
         <v>58</v>
       </c>
       <c r="C180" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="D180" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="E180" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="F180" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="G180" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="H180" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="I180" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="J180" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="K180" s="101">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="L180" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="M180" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="N180" s="102">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="O180" s="59">
-        <v>0.0192307692307692</v>
+        <v>0.019230769230769232</v>
       </c>
       <c r="P180" s="105" t="s">
         <v>38</v>
@@ -8315,46 +8044,46 @@
         <v>59</v>
       </c>
       <c r="C182" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="D182" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="E182" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="F182" s="109">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="G182" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="H182" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="I182" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="J182" s="109">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="K182" s="103">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="L182" s="95">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="M182" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="N182" s="108">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="O182" s="98">
-        <v>384.615384615385</v>
+        <v>384.61538461538464</v>
       </c>
       <c r="P182" s="98">
-        <v>5000.0000000000036</v>
+        <v>5000.0000000000009</v>
       </c>
     </row>
     <row r="183" ht="24" customHeight="1">
@@ -8472,7 +8201,851 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" ht="24" customHeight="1" s="94" customFormat="1"/>
+    <row r="187">
+      <c r="A187" s="57"/>
+      <c r="B187" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="C187" s="133" t="s">
+        <v>83</v>
+      </c>
+      <c r="D187" s="133"/>
+      <c r="E187" s="133"/>
+      <c r="F187" s="134"/>
+      <c r="G187" s="133" t="s">
+        <v>84</v>
+      </c>
+      <c r="H187" s="133"/>
+      <c r="I187" s="133"/>
+      <c r="J187" s="134"/>
+      <c r="K187" s="135" t="s">
+        <v>85</v>
+      </c>
+      <c r="L187" s="133"/>
+      <c r="M187" s="133"/>
+      <c r="N187" s="133"/>
+      <c r="O187" s="134"/>
+      <c r="P187" s="32"/>
+    </row>
+    <row r="188" ht="24" customHeight="1">
+      <c r="A188" s="57"/>
+      <c r="B188" s="66"/>
+      <c r="C188" s="55">
+        <v>43920</v>
+      </c>
+      <c r="D188" s="55">
+        <v>43927</v>
+      </c>
+      <c r="E188" s="55">
+        <v>43934</v>
+      </c>
+      <c r="F188" s="56">
+        <v>43941</v>
+      </c>
+      <c r="G188" s="55">
+        <v>43948</v>
+      </c>
+      <c r="H188" s="55">
+        <v>43955</v>
+      </c>
+      <c r="I188" s="55">
+        <v>43962</v>
+      </c>
+      <c r="J188" s="56">
+        <v>43969</v>
+      </c>
+      <c r="K188" s="55">
+        <v>43976</v>
+      </c>
+      <c r="L188" s="55">
+        <v>43983</v>
+      </c>
+      <c r="M188" s="55">
+        <v>43990</v>
+      </c>
+      <c r="N188" s="55">
+        <v>43997</v>
+      </c>
+      <c r="O188" s="56">
+        <v>44004</v>
+      </c>
+      <c r="P188" s="60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="189" ht="24" customHeight="1">
+      <c r="B189" s="114" t="s">
+        <v>58</v>
+      </c>
+      <c r="C189" s="101">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="D189" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="E189" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="F189" s="59">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="G189" s="101">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="H189" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="I189" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="J189" s="59">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="K189" s="101">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="L189" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="M189" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="N189" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="O189" s="59">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="P189" s="105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="190" ht="24" customHeight="1">
+      <c r="B190" s="115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C190" s="104">
+        <v>0</v>
+      </c>
+      <c r="D190" s="96">
+        <v>0</v>
+      </c>
+      <c r="E190" s="106">
+        <v>0</v>
+      </c>
+      <c r="F190" s="107">
+        <v>0</v>
+      </c>
+      <c r="G190" s="104">
+        <v>0</v>
+      </c>
+      <c r="H190" s="96">
+        <v>0</v>
+      </c>
+      <c r="I190" s="106">
+        <v>0</v>
+      </c>
+      <c r="J190" s="107">
+        <v>0</v>
+      </c>
+      <c r="K190" s="104">
+        <v>0</v>
+      </c>
+      <c r="L190" s="96">
+        <v>0</v>
+      </c>
+      <c r="M190" s="106">
+        <v>0</v>
+      </c>
+      <c r="N190" s="106">
+        <v>0</v>
+      </c>
+      <c r="O190" s="99">
+        <v>0</v>
+      </c>
+      <c r="P190" s="99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" ht="24" customHeight="1">
+      <c r="B191" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="C191" s="103">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="D191" s="95">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="E191" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="F191" s="109">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="G191" s="103">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="H191" s="95">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="I191" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="J191" s="109">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="K191" s="103">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="L191" s="95">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="M191" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="N191" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="O191" s="98">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="P191" s="98">
+        <v>5000.0000000000009</v>
+      </c>
+    </row>
+    <row r="192" ht="24" customHeight="1">
+      <c r="B192" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="C192" s="110">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="D192" s="97">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="E192" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="F192" s="112">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="G192" s="110">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="H192" s="97">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="I192" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="J192" s="112">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="K192" s="110">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="L192" s="97">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="M192" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="N192" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="O192" s="113">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="P192" s="113">
+        <v>24.999999999999957</v>
+      </c>
+    </row>
+    <row r="193" ht="24" customHeight="1">
+      <c r="B193" s="115" t="s">
+        <v>60</v>
+      </c>
+      <c r="C193" s="61">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="D193" s="62">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="E193" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="F193" s="65">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="G193" s="61">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="H193" s="62">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="I193" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="J193" s="65">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="K193" s="61">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="L193" s="62">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="M193" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="N193" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="O193" s="63">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="P193" s="63">
+        <v>124999.9999999998</v>
+      </c>
+    </row>
+    <row r="194" ht="30" customHeight="1">
+      <c r="B194" s="116" t="s">
+        <v>61</v>
+      </c>
+      <c r="C194" s="117"/>
+      <c r="D194" s="118"/>
+      <c r="E194" s="118"/>
+      <c r="F194" s="118"/>
+      <c r="G194" s="117"/>
+      <c r="H194" s="118"/>
+      <c r="I194" s="118"/>
+      <c r="J194" s="119"/>
+      <c r="K194" s="117"/>
+      <c r="L194" s="118"/>
+      <c r="M194" s="118"/>
+      <c r="N194" s="118"/>
+      <c r="O194" s="119"/>
+      <c r="P194" s="120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="57"/>
+      <c r="B196" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C196" s="133" t="s">
+        <v>83</v>
+      </c>
+      <c r="D196" s="133"/>
+      <c r="E196" s="133"/>
+      <c r="F196" s="134"/>
+      <c r="G196" s="133" t="s">
+        <v>84</v>
+      </c>
+      <c r="H196" s="133"/>
+      <c r="I196" s="133"/>
+      <c r="J196" s="134"/>
+      <c r="K196" s="135" t="s">
+        <v>85</v>
+      </c>
+      <c r="L196" s="133"/>
+      <c r="M196" s="133"/>
+      <c r="N196" s="133"/>
+      <c r="O196" s="134"/>
+      <c r="P196" s="32"/>
+    </row>
+    <row r="197" ht="24" customHeight="1">
+      <c r="A197" s="57"/>
+      <c r="B197" s="66"/>
+      <c r="C197" s="55">
+        <v>43920</v>
+      </c>
+      <c r="D197" s="55">
+        <v>43927</v>
+      </c>
+      <c r="E197" s="55">
+        <v>43934</v>
+      </c>
+      <c r="F197" s="56">
+        <v>43941</v>
+      </c>
+      <c r="G197" s="55">
+        <v>43948</v>
+      </c>
+      <c r="H197" s="55">
+        <v>43955</v>
+      </c>
+      <c r="I197" s="55">
+        <v>43962</v>
+      </c>
+      <c r="J197" s="56">
+        <v>43969</v>
+      </c>
+      <c r="K197" s="55">
+        <v>43976</v>
+      </c>
+      <c r="L197" s="55">
+        <v>43983</v>
+      </c>
+      <c r="M197" s="55">
+        <v>43990</v>
+      </c>
+      <c r="N197" s="55">
+        <v>43997</v>
+      </c>
+      <c r="O197" s="56">
+        <v>44004</v>
+      </c>
+      <c r="P197" s="60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="198" ht="24" customHeight="1">
+      <c r="B198" s="114" t="s">
+        <v>58</v>
+      </c>
+      <c r="C198" s="101">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="D198" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="E198" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="F198" s="59">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="G198" s="101">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="H198" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="I198" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="J198" s="59">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="K198" s="101">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="L198" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="M198" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="N198" s="102">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="O198" s="59">
+        <v>0.019230769230769232</v>
+      </c>
+      <c r="P198" s="105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="199" ht="24" customHeight="1">
+      <c r="B199" s="115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C199" s="104">
+        <v>0</v>
+      </c>
+      <c r="D199" s="96">
+        <v>0</v>
+      </c>
+      <c r="E199" s="106">
+        <v>0</v>
+      </c>
+      <c r="F199" s="107">
+        <v>0</v>
+      </c>
+      <c r="G199" s="104">
+        <v>0</v>
+      </c>
+      <c r="H199" s="96">
+        <v>0</v>
+      </c>
+      <c r="I199" s="106">
+        <v>0</v>
+      </c>
+      <c r="J199" s="107">
+        <v>0</v>
+      </c>
+      <c r="K199" s="104">
+        <v>0</v>
+      </c>
+      <c r="L199" s="96">
+        <v>0</v>
+      </c>
+      <c r="M199" s="106">
+        <v>0</v>
+      </c>
+      <c r="N199" s="106">
+        <v>0</v>
+      </c>
+      <c r="O199" s="99">
+        <v>0</v>
+      </c>
+      <c r="P199" s="99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" ht="24" customHeight="1">
+      <c r="B200" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="C200" s="103">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="D200" s="95">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="E200" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="F200" s="109">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="G200" s="103">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="H200" s="95">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="I200" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="J200" s="109">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="K200" s="103">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="L200" s="95">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="M200" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="N200" s="108">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="O200" s="98">
+        <v>384.61538461538464</v>
+      </c>
+      <c r="P200" s="98">
+        <v>5000.0000000000009</v>
+      </c>
+    </row>
+    <row r="201" ht="24" customHeight="1">
+      <c r="B201" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="C201" s="110">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="D201" s="97">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="E201" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="F201" s="112">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="G201" s="110">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="H201" s="97">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="I201" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="J201" s="112">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="K201" s="110">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="L201" s="97">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="M201" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="N201" s="111">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="O201" s="113">
+        <v>24.999999999999936</v>
+      </c>
+      <c r="P201" s="113">
+        <v>24.999999999999957</v>
+      </c>
+    </row>
+    <row r="202" ht="24" customHeight="1">
+      <c r="B202" s="115" t="s">
+        <v>60</v>
+      </c>
+      <c r="C202" s="61">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="D202" s="62">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="E202" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="F202" s="65">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="G202" s="61">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="H202" s="62">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="I202" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="J202" s="65">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="K202" s="61">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="L202" s="62">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="M202" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="N202" s="64">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="O202" s="63">
+        <v>9615.3846153846</v>
+      </c>
+      <c r="P202" s="63">
+        <v>124999.9999999998</v>
+      </c>
+    </row>
+    <row r="203" ht="30" customHeight="1">
+      <c r="B203" s="116" t="s">
+        <v>61</v>
+      </c>
+      <c r="C203" s="117"/>
+      <c r="D203" s="118"/>
+      <c r="E203" s="118"/>
+      <c r="F203" s="118"/>
+      <c r="G203" s="117"/>
+      <c r="H203" s="118"/>
+      <c r="I203" s="118"/>
+      <c r="J203" s="119"/>
+      <c r="K203" s="117"/>
+      <c r="L203" s="118"/>
+      <c r="M203" s="118"/>
+      <c r="N203" s="118"/>
+      <c r="O203" s="119"/>
+      <c r="P203" s="120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="57"/>
+      <c r="B205" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="C205" s="133" t="s">
+        <v>83</v>
+      </c>
+      <c r="D205" s="133"/>
+      <c r="E205" s="133"/>
+      <c r="F205" s="134"/>
+      <c r="G205" s="133" t="s">
+        <v>84</v>
+      </c>
+      <c r="H205" s="133"/>
+      <c r="I205" s="133"/>
+      <c r="J205" s="134"/>
+      <c r="K205" s="135" t="s">
+        <v>85</v>
+      </c>
+      <c r="L205" s="133"/>
+      <c r="M205" s="133"/>
+      <c r="N205" s="133"/>
+      <c r="O205" s="134"/>
+      <c r="P205" s="32"/>
+    </row>
+    <row r="206" ht="24" customHeight="1">
+      <c r="A206" s="57"/>
+      <c r="B206" s="66"/>
+      <c r="C206" s="55">
+        <v>43920</v>
+      </c>
+      <c r="D206" s="55">
+        <v>43927</v>
+      </c>
+      <c r="E206" s="55">
+        <v>43934</v>
+      </c>
+      <c r="F206" s="56">
+        <v>43941</v>
+      </c>
+      <c r="G206" s="55">
+        <v>43948</v>
+      </c>
+      <c r="H206" s="55">
+        <v>43955</v>
+      </c>
+      <c r="I206" s="55">
+        <v>43962</v>
+      </c>
+      <c r="J206" s="56">
+        <v>43969</v>
+      </c>
+      <c r="K206" s="55">
+        <v>43976</v>
+      </c>
+      <c r="L206" s="55">
+        <v>43983</v>
+      </c>
+      <c r="M206" s="55">
+        <v>43990</v>
+      </c>
+      <c r="N206" s="55">
+        <v>43997</v>
+      </c>
+      <c r="O206" s="56">
+        <v>44004</v>
+      </c>
+      <c r="P206" s="60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="207" ht="24" customHeight="1">
+      <c r="B207" s="114" t="s">
+        <v>58</v>
+      </c>
+      <c r="C207" s="101"/>
+      <c r="D207" s="102"/>
+      <c r="E207" s="102"/>
+      <c r="F207" s="59"/>
+      <c r="G207" s="101"/>
+      <c r="H207" s="102"/>
+      <c r="I207" s="102"/>
+      <c r="J207" s="59"/>
+      <c r="K207" s="101"/>
+      <c r="L207" s="102"/>
+      <c r="M207" s="102"/>
+      <c r="N207" s="102"/>
+      <c r="O207" s="59"/>
+      <c r="P207" s="105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="208" ht="24" customHeight="1">
+      <c r="B208" s="115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C208" s="104"/>
+      <c r="D208" s="96"/>
+      <c r="E208" s="106"/>
+      <c r="F208" s="107"/>
+      <c r="G208" s="104"/>
+      <c r="H208" s="96"/>
+      <c r="I208" s="106"/>
+      <c r="J208" s="107"/>
+      <c r="K208" s="104"/>
+      <c r="L208" s="96"/>
+      <c r="M208" s="106"/>
+      <c r="N208" s="106"/>
+      <c r="O208" s="99"/>
+      <c r="P208" s="99"/>
+    </row>
+    <row r="209" ht="24" customHeight="1">
+      <c r="B209" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="C209" s="103"/>
+      <c r="D209" s="95"/>
+      <c r="E209" s="108"/>
+      <c r="F209" s="109"/>
+      <c r="G209" s="103"/>
+      <c r="H209" s="95"/>
+      <c r="I209" s="108"/>
+      <c r="J209" s="109"/>
+      <c r="K209" s="103"/>
+      <c r="L209" s="95"/>
+      <c r="M209" s="108"/>
+      <c r="N209" s="108"/>
+      <c r="O209" s="98"/>
+      <c r="P209" s="98"/>
+    </row>
+    <row r="210" ht="24" customHeight="1">
+      <c r="B210" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="C210" s="110"/>
+      <c r="D210" s="97"/>
+      <c r="E210" s="111"/>
+      <c r="F210" s="112"/>
+      <c r="G210" s="110"/>
+      <c r="H210" s="97"/>
+      <c r="I210" s="111"/>
+      <c r="J210" s="112"/>
+      <c r="K210" s="110"/>
+      <c r="L210" s="97"/>
+      <c r="M210" s="111"/>
+      <c r="N210" s="111"/>
+      <c r="O210" s="113"/>
+      <c r="P210" s="113"/>
+    </row>
+    <row r="211" ht="24" customHeight="1">
+      <c r="B211" s="115" t="s">
+        <v>60</v>
+      </c>
+      <c r="C211" s="61"/>
+      <c r="D211" s="62"/>
+      <c r="E211" s="64"/>
+      <c r="F211" s="65"/>
+      <c r="G211" s="61"/>
+      <c r="H211" s="62"/>
+      <c r="I211" s="64"/>
+      <c r="J211" s="65"/>
+      <c r="K211" s="61"/>
+      <c r="L211" s="62"/>
+      <c r="M211" s="64"/>
+      <c r="N211" s="64"/>
+      <c r="O211" s="63"/>
+      <c r="P211" s="63"/>
+    </row>
+    <row r="212" ht="30" customHeight="1">
+      <c r="B212" s="116" t="s">
+        <v>61</v>
+      </c>
+      <c r="C212" s="117"/>
+      <c r="D212" s="118"/>
+      <c r="E212" s="118"/>
+      <c r="F212" s="118"/>
+      <c r="G212" s="117"/>
+      <c r="H212" s="118"/>
+      <c r="I212" s="118"/>
+      <c r="J212" s="119"/>
+      <c r="K212" s="117"/>
+      <c r="L212" s="118"/>
+      <c r="M212" s="118"/>
+      <c r="N212" s="118"/>
+      <c r="O212" s="119"/>
+      <c r="P212" s="120"/>
+    </row>
+    <row r="213" ht="24" customHeight="1" s="94" customFormat="1"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="D5:P5"/>
@@ -8536,6 +9109,15 @@
     <mergeCell ref="C178:F178"/>
     <mergeCell ref="G178:J178"/>
     <mergeCell ref="K178:O178"/>
+    <mergeCell ref="C187:F187"/>
+    <mergeCell ref="G187:J187"/>
+    <mergeCell ref="K187:O187"/>
+    <mergeCell ref="C196:F196"/>
+    <mergeCell ref="G196:J196"/>
+    <mergeCell ref="K196:O196"/>
+    <mergeCell ref="C205:F205"/>
+    <mergeCell ref="G205:J205"/>
+    <mergeCell ref="K205:O205"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
     <cfRule type="expression" dxfId="0" priority="3">
@@ -8640,7 +9222,7 @@
         <v>14</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>16</v>
@@ -8673,7 +9255,7 @@
     </row>
     <row r="7" ht="24" customHeight="1">
       <c r="B7" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -8934,7 +9516,7 @@
     </row>
     <row r="13" ht="24" customHeight="1">
       <c r="B13" s="52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -11197,10 +11779,10 @@
     <row r="2" ht="24" customHeight="1">
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -11235,25 +11817,25 @@
     </row>
     <row r="5" ht="18" customHeight="1" s="5" customFormat="1">
       <c r="C5" s="130" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D5" s="130"/>
       <c r="E5" s="130" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F5" s="130"/>
       <c r="G5" s="130"/>
       <c r="H5" s="73"/>
       <c r="I5" s="130" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J5" s="130"/>
       <c r="K5" s="130" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L5" s="130"/>
       <c r="M5" s="130" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="N5" s="130"/>
       <c r="O5" s="68" t="s">
@@ -11285,7 +11867,7 @@
     </row>
     <row r="7" ht="24" customHeight="1">
       <c r="C7" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D7" s="52"/>
       <c r="E7" s="9"/>
@@ -11301,7 +11883,7 @@
       <c r="M7" s="133"/>
       <c r="N7" s="134"/>
       <c r="O7" s="135" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="P7" s="133"/>
       <c r="Q7" s="133"/>
@@ -11312,14 +11894,14 @@
     </row>
     <row r="8" ht="24" customHeight="1">
       <c r="A8" s="72" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="38" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>23</v>
@@ -11373,14 +11955,14 @@
     </row>
     <row r="9" ht="24" customHeight="1">
       <c r="A9" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E9" s="77">
         <v>0</v>
@@ -11434,14 +12016,14 @@
     </row>
     <row r="10" ht="24" customHeight="1">
       <c r="A10" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E10" s="77">
         <v>0</v>
@@ -11495,14 +12077,14 @@
     </row>
     <row r="11" ht="24" customHeight="1">
       <c r="A11" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E11" s="77">
         <v>0</v>
@@ -11556,14 +12138,14 @@
     </row>
     <row r="12" ht="24" customHeight="1">
       <c r="A12" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E12" s="77">
         <v>0</v>
@@ -11617,14 +12199,14 @@
     </row>
     <row r="13" ht="24" customHeight="1">
       <c r="A13" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E13" s="77">
         <v>0</v>
@@ -11680,7 +12262,7 @@
       <c r="B14" s="27"/>
       <c r="C14" s="38"/>
       <c r="D14" s="39" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E14" s="50">
         <v>0</v>
@@ -11738,13 +12320,13 @@
     <row r="16" ht="24" customHeight="1" s="74" customFormat="1">
       <c r="B16" s="57"/>
       <c r="H16" s="84" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" ht="24" customHeight="1" s="74" customFormat="1">
       <c r="B17" s="57"/>
       <c r="H17" s="135" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I17" s="133"/>
       <c r="J17" s="133"/>
@@ -11807,7 +12389,7 @@
     </row>
     <row r="19" ht="24" customHeight="1" s="74" customFormat="1">
       <c r="A19" s="74" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B19" s="57"/>
       <c r="H19" s="128">
@@ -11841,7 +12423,7 @@
     </row>
     <row r="20" ht="24" customHeight="1">
       <c r="A20" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B20" s="57"/>
       <c r="H20" s="128">
@@ -11875,7 +12457,7 @@
     </row>
     <row r="21" ht="24" customHeight="1">
       <c r="A21" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B21" s="57"/>
       <c r="H21" s="128">
@@ -11909,7 +12491,7 @@
     </row>
     <row r="22" ht="24" customHeight="1">
       <c r="A22" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B22" s="57"/>
       <c r="H22" s="128">
@@ -11943,7 +12525,7 @@
     </row>
     <row r="23" ht="24" customHeight="1">
       <c r="A23" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B23" s="57"/>
       <c r="H23" s="128">
@@ -12047,7 +12629,7 @@
     </row>
     <row r="28" ht="24" customHeight="1">
       <c r="C28" s="52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D28" s="52"/>
       <c r="E28" s="9"/>
@@ -12063,7 +12645,7 @@
       <c r="M28" s="133"/>
       <c r="N28" s="134"/>
       <c r="O28" s="135" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="P28" s="133"/>
       <c r="Q28" s="133"/>
@@ -12074,14 +12656,14 @@
     </row>
     <row r="29" ht="24" customHeight="1">
       <c r="A29" s="72" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="38" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E29" s="39" t="s">
         <v>23</v>
@@ -12135,14 +12717,14 @@
     </row>
     <row r="30" ht="24" customHeight="1">
       <c r="A30" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E30" s="77">
         <v>0</v>
@@ -12196,14 +12778,14 @@
     </row>
     <row r="31" ht="24" customHeight="1">
       <c r="A31" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="10" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E31" s="77">
         <v>0</v>
@@ -12257,14 +12839,14 @@
     </row>
     <row r="32" ht="24" customHeight="1">
       <c r="A32" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B32" s="27"/>
       <c r="C32" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E32" s="77">
         <v>0</v>
@@ -12318,14 +12900,14 @@
     </row>
     <row r="33" ht="24" customHeight="1">
       <c r="A33" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B33" s="27"/>
       <c r="C33" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E33" s="77">
         <v>0</v>
@@ -12381,7 +12963,7 @@
       <c r="B34" s="27"/>
       <c r="C34" s="38"/>
       <c r="D34" s="39" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E34" s="50">
         <v>0</v>
@@ -12435,7 +13017,7 @@
     </row>
     <row r="36" ht="24" customHeight="1">
       <c r="C36" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D36" s="52"/>
       <c r="E36" s="9"/>
@@ -12451,7 +13033,7 @@
       <c r="M36" s="133"/>
       <c r="N36" s="134"/>
       <c r="O36" s="135" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="P36" s="133"/>
       <c r="Q36" s="133"/>
@@ -12462,14 +13044,14 @@
     </row>
     <row r="37" ht="24" customHeight="1">
       <c r="A37" s="72" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B37" s="27"/>
       <c r="C37" s="38" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E37" s="39" t="s">
         <v>23</v>
@@ -12523,14 +13105,14 @@
     </row>
     <row r="38" ht="24" customHeight="1">
       <c r="A38" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B38" s="27"/>
       <c r="C38" s="10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E38" s="77">
         <v>0</v>
@@ -12584,14 +13166,14 @@
     </row>
     <row r="39" ht="24" customHeight="1">
       <c r="A39" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B39" s="27"/>
       <c r="C39" s="10" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E39" s="77">
         <v>0</v>
@@ -12647,7 +13229,7 @@
       <c r="B40" s="27"/>
       <c r="C40" s="38"/>
       <c r="D40" s="39" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E40" s="50">
         <v>0</v>
@@ -12717,7 +13299,7 @@
       <c r="M42" s="133"/>
       <c r="N42" s="134"/>
       <c r="O42" s="135" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="P42" s="133"/>
       <c r="Q42" s="133"/>
@@ -12728,14 +13310,14 @@
     </row>
     <row r="43" ht="24" customHeight="1">
       <c r="A43" s="72" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B43" s="27"/>
       <c r="C43" s="38" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E43" s="39" t="s">
         <v>23</v>
@@ -12789,14 +13371,14 @@
     </row>
     <row r="44" ht="24" customHeight="1">
       <c r="A44" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B44" s="27"/>
       <c r="C44" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E44" s="77">
         <v>0</v>
@@ -12850,14 +13432,14 @@
     </row>
     <row r="45" ht="24" customHeight="1">
       <c r="A45" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B45" s="27"/>
       <c r="C45" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E45" s="77">
         <v>0</v>
@@ -12911,14 +13493,14 @@
     </row>
     <row r="46" ht="24" customHeight="1">
       <c r="A46" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B46" s="27"/>
       <c r="C46" s="10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E46" s="77">
         <v>0</v>
@@ -12972,14 +13554,14 @@
     </row>
     <row r="47" ht="24" customHeight="1">
       <c r="A47" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B47" s="27"/>
       <c r="C47" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E47" s="77">
         <v>0</v>
@@ -13033,14 +13615,14 @@
     </row>
     <row r="48" ht="24" customHeight="1">
       <c r="A48" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B48" s="27"/>
       <c r="C48" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E48" s="77">
         <v>0</v>
@@ -13094,14 +13676,14 @@
     </row>
     <row r="49" ht="24" customHeight="1">
       <c r="A49" s="72" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B49" s="27"/>
       <c r="C49" s="10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E49" s="77">
         <v>0</v>
@@ -13155,14 +13737,14 @@
     </row>
     <row r="50" ht="24" customHeight="1">
       <c r="A50" s="72" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B50" s="27"/>
       <c r="C50" s="10" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E50" s="77">
         <v>0</v>
@@ -13218,7 +13800,7 @@
       <c r="B51" s="27"/>
       <c r="C51" s="38"/>
       <c r="D51" s="39" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E51" s="50">
         <v>0</v>
@@ -13278,7 +13860,7 @@
       <c r="D53" s="54"/>
       <c r="E53" s="75"/>
       <c r="F53" s="140" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G53" s="140"/>
       <c r="H53" s="140"/>
@@ -13324,7 +13906,7 @@
       </c>
       <c r="D55" s="54"/>
       <c r="F55" s="140" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G55" s="140"/>
       <c r="H55" s="140"/>
@@ -13370,7 +13952,7 @@
       <c r="D57" s="54"/>
       <c r="E57" s="75"/>
       <c r="F57" s="140" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G57" s="140"/>
       <c r="H57" s="140"/>
@@ -13459,7 +14041,7 @@
       </c>
       <c r="D61" s="54"/>
       <c r="F61" s="131" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G61" s="131"/>
       <c r="H61" s="131"/>

</xml_diff>

<commit_message>
Merged PR 7467: PRI-21224 Export Campaign to Excel - Dayparts - Implement Flight Days
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/Stub Advertiser DAY EMN MDN PA PT Q4'19-Q2'20 Plan Rev - 12-16.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/Stub Advertiser DAY EMN MDN PA PT Q4'19-Q2'20 Plan Rev - 12-16.xlsx
@@ -316,7 +316,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 02/14/20</t>
+    <t>Created 02/19/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -382,7 +382,7 @@
     <t>~80% Minimum TV HH Coverage</t>
   </si>
   <si>
-    <t>DAY - 09:00am - 04:00pm, EMN - 04:00am - 10:00am, MDN - 11:00am - 01:00pm, PA - 06:00pm - 08:00pm, PT - 08:00pm - 11:00pm</t>
+    <t>DAY - M-SU 09:00am - 04:00pm, EMN - M-SU 04:00am - 10:00am, MDN - M-F,SU 11:00am - 01:00pm, PA - M-F,SU 06:00pm - 08:00pm, PT - M-SU 08:00pm - 11:00pm</t>
   </si>
   <si>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">

</xml_diff>